<commit_message>
Update Stand-up file name
</commit_message>
<xml_diff>
--- a/Documents/Stand-up Document Week 12.xlsx
+++ b/Documents/Stand-up Document Week 12.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/Team-WeChat-new/Documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Group Member</t>
   </si>
@@ -154,47 +170,70 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <u/>
-      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF00A2FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -202,7 +241,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -224,37 +263,61 @@
     </fill>
   </fills>
   <borders count="7">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -264,99 +327,337 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.14"/>
-    <col customWidth="1" min="2" max="2" width="20.0"/>
-    <col customWidth="1" min="3" max="3" width="38.29"/>
-    <col customWidth="1" min="4" max="4" width="41.57"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" customWidth="1"/>
+    <col min="4" max="4" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -392,7 +693,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -428,7 +729,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8" t="s">
@@ -438,7 +739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
@@ -470,7 +771,7 @@
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -484,7 +785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
@@ -514,7 +815,7 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
@@ -528,7 +829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="s">
@@ -538,7 +839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
@@ -570,7 +871,7 @@
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
@@ -584,7 +885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="s">
@@ -594,7 +895,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
@@ -626,7 +927,7 @@
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
@@ -640,7 +941,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
@@ -672,7 +973,7 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>4</v>
       </c>
@@ -686,7 +987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19" t="s">
@@ -696,7 +997,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21" t="s">
@@ -706,7 +1007,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="22" t="s">
         <v>27</v>
       </c>
@@ -716,17 +1017,19 @@
       <c r="C18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
+      <c r="D18" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="20"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="22" t="s">
         <v>11</v>
       </c>
@@ -740,9 +1043,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="21" t="s">
         <v>40</v>
       </c>
@@ -750,7 +1053,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="22" t="s">
         <v>42</v>
       </c>
@@ -760,19 +1063,19 @@
       <c r="C22" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="21"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="s">
         <v>15</v>
       </c>
@@ -782,36 +1085,37 @@
       <c r="C24" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D2"/>
-    <hyperlink r:id="rId2" ref="D3"/>
-    <hyperlink r:id="rId3" ref="D4"/>
-    <hyperlink r:id="rId4" ref="D5"/>
-    <hyperlink r:id="rId5" ref="D7"/>
-    <hyperlink r:id="rId6" ref="D8"/>
-    <hyperlink r:id="rId7" ref="D9"/>
-    <hyperlink r:id="rId8" ref="D10"/>
-    <hyperlink r:id="rId9" ref="D11"/>
-    <hyperlink r:id="rId10" ref="D12"/>
-    <hyperlink r:id="rId11" ref="D13"/>
-    <hyperlink r:id="rId12" ref="D14"/>
-    <hyperlink r:id="rId13" ref="D15"/>
-    <hyperlink r:id="rId14" ref="D16"/>
-    <hyperlink r:id="rId15" ref="D17"/>
-    <hyperlink r:id="rId16" ref="D22"/>
-    <hyperlink r:id="rId17" ref="D24"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D14" r:id="rId12"/>
+    <hyperlink ref="D15" r:id="rId13"/>
+    <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="D17" r:id="rId15"/>
+    <hyperlink ref="D24" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D18" r:id="rId18"/>
   </hyperlinks>
-  <drawing r:id="rId18"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>